<commit_message>
Import of JANDREW/Spreadsheet-XLSX-Reader-LibXML-v0.22.2.tar.gz from CPAN.
gitpan-cpan-distribution: Spreadsheet-XLSX-Reader-LibXML
gitpan-cpan-version:      v0.22.2
gitpan-cpan-path:         JANDREW/Spreadsheet-XLSX-Reader-LibXML-v0.22.2.tar.gz
gitpan-cpan-author:       JANDREW
gitpan-cpan-maturity:     released
</commit_message>
<xml_diff>
--- a/t/test_files/TestBook.xlsx
+++ b/t/test_files/TestBook.xlsx
@@ -698,7 +698,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -807,7 +807,7 @@
   <dimension ref="A2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -859,7 +859,7 @@
       <c r="E10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Import of JANDREW/Spreadsheet-XLSX-Reader-LibXML-v0.24.2.tar.gz from CPAN.
gitpan-cpan-distribution: Spreadsheet-XLSX-Reader-LibXML
gitpan-cpan-version:      v0.24.2
gitpan-cpan-path:         JANDREW/Spreadsheet-XLSX-Reader-LibXML-v0.24.2.tar.gz
gitpan-cpan-author:       JANDREW
gitpan-cpan-maturity:     released
</commit_message>
<xml_diff>
--- a/t/test_files/TestBook.xlsx
+++ b/t/test_files/TestBook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="15150" windowHeight="4455" tabRatio="505" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="9345" windowHeight="4455" tabRatio="505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -807,7 +807,7 @@
   <dimension ref="A2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -869,6 +869,10 @@
       </c>
     </row>
     <row r="12" spans="1:6">
+      <c r="B12" t="str">
+        <f>IF(B11&gt;0,"Hello","")</f>
+        <v/>
+      </c>
       <c r="D12" s="10">
         <f>DATEVALUE(E10)</f>
         <v>39118</v>

</xml_diff>